<commit_message>
add confirmed cases in hospital
</commit_message>
<xml_diff>
--- a/huanggang/20200129.xlsx
+++ b/huanggang/20200129.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouzhengxi/Downloads/2019-nCoV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouzhengxi/Programming/github/zzxwill/2019-nCoV/huanggang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9416A744-3053-1547-B859-9F60D2267AF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18540" yWindow="1260" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -107,8 +114,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -119,6 +126,11 @@
       <sz val="11.5"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -473,11 +485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -559,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -634,7 +646,7 @@
         <v>52</v>
       </c>
       <c r="C11" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
@@ -692,6 +704,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="1.25" right="1.25" top="1" bottom="0.79166666666666696" header="0.25" footer="0.25"/>
 </worksheet>
 </file>
</xml_diff>